<commit_message>
add Students_Table class and example use; add convert_string_to_s32
</commit_message>
<xml_diff>
--- a/final_project/school_journal/database/excel.xlsx
+++ b/final_project/school_journal/database/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\school_journal\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346C943B-0F21-4CBB-A4CD-111AF0A10C3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C127E80-C6B5-4E7C-891F-DA6768DBC831}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="-120" windowWidth="27975" windowHeight="16440" tabRatio="790" activeTab="3" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-27855" yWindow="-120" windowWidth="27975" windowHeight="16440" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4C6B96-C4DC-4735-B81E-35A8CA1960AC}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -881,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1051,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1493,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BBAA83-CB17-480D-9BF2-9E6FB44F98AF}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
discard Table class; add class for every database element
</commit_message>
<xml_diff>
--- a/final_project/school_journal/database/excel.xlsx
+++ b/final_project/school_journal/database/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\school_journal\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C127E80-C6B5-4E7C-891F-DA6768DBC831}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DC146B-A79E-4A78-B34C-C13AC74C346D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27855" yWindow="-120" windowWidth="27975" windowHeight="16440" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-27720" yWindow="0" windowWidth="22395" windowHeight="13170" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,8 @@
     <sheet name="Fields of study" sheetId="2" r:id="rId3"/>
     <sheet name="Grades" sheetId="5" r:id="rId4"/>
     <sheet name="Grades comments" sheetId="8" r:id="rId5"/>
-    <sheet name="Suspended students" sheetId="9" r:id="rId6"/>
-    <sheet name="Instructors" sheetId="4" r:id="rId7"/>
-    <sheet name="Enrollments" sheetId="6" r:id="rId8"/>
+    <sheet name="Instructors" sheetId="4" r:id="rId6"/>
+    <sheet name="Enrollments" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>Index</t>
   </si>
@@ -317,15 +316,6 @@
   </si>
   <si>
     <t>Some comment.</t>
-  </si>
-  <si>
-    <t>Reason</t>
-  </si>
-  <si>
-    <t>Some reason…</t>
-  </si>
-  <si>
-    <t>ECTS_deficit</t>
   </si>
   <si>
     <t>Short_name</t>
@@ -766,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4C6B96-C4DC-4735-B81E-35A8CA1960AC}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +772,7 @@
     <col min="10" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -793,13 +783,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100100</v>
       </c>
@@ -812,11 +799,8 @@
       <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100101</v>
       </c>
@@ -829,11 +813,8 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100102</v>
       </c>
@@ -846,11 +827,8 @@
       <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100103</v>
       </c>
@@ -863,11 +841,8 @@
       <c r="D5" s="7">
         <v>3</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100104</v>
       </c>
@@ -880,11 +855,8 @@
       <c r="D6" s="7">
         <v>3</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>100105</v>
       </c>
@@ -897,11 +869,8 @@
       <c r="D7" s="7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100106</v>
       </c>
@@ -914,11 +883,8 @@
       <c r="D8" s="7">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>100107</v>
       </c>
@@ -931,11 +897,8 @@
       <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100108</v>
       </c>
@@ -948,11 +911,8 @@
       <c r="D10" s="7">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100109</v>
       </c>
@@ -965,11 +925,8 @@
       <c r="D11" s="7">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>100110</v>
       </c>
@@ -982,11 +939,8 @@
       <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>100111</v>
       </c>
@@ -999,11 +953,8 @@
       <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100112</v>
       </c>
@@ -1016,11 +967,8 @@
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>100113</v>
       </c>
@@ -1033,11 +981,8 @@
       <c r="D15" s="7">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>100114</v>
       </c>
@@ -1050,11 +995,8 @@
       <c r="D16" s="7">
         <v>2</v>
       </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>100115</v>
       </c>
@@ -1067,11 +1009,8 @@
       <c r="D17" s="7">
         <v>3</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>100116</v>
       </c>
@@ -1084,11 +1023,8 @@
       <c r="D18" s="7">
         <v>3</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>100117</v>
       </c>
@@ -1101,11 +1037,8 @@
       <c r="D19" s="7">
         <v>2</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>100118</v>
       </c>
@@ -1118,11 +1051,8 @@
       <c r="D20" s="7">
         <v>1</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>100119</v>
       </c>
@@ -1135,11 +1065,8 @@
       <c r="D21" s="7">
         <v>3</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>100120</v>
       </c>
@@ -1152,11 +1079,8 @@
       <c r="D22" s="7">
         <v>3</v>
       </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>100121</v>
       </c>
@@ -1169,11 +1093,8 @@
       <c r="D23" s="7">
         <v>1</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>100122</v>
       </c>
@@ -1186,11 +1107,8 @@
       <c r="D24" s="7">
         <v>2</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>100123</v>
       </c>
@@ -1203,11 +1121,8 @@
       <c r="D25" s="7">
         <v>2</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>100124</v>
       </c>
@@ -1220,11 +1135,8 @@
       <c r="D26" s="7">
         <v>3</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>100125</v>
       </c>
@@ -1237,11 +1149,8 @@
       <c r="D27" s="7">
         <v>1</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>100126</v>
       </c>
@@ -1254,11 +1163,8 @@
       <c r="D28" s="7">
         <v>3</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>100127</v>
       </c>
@@ -1271,11 +1177,8 @@
       <c r="D29" s="7">
         <v>3</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>100128</v>
       </c>
@@ -1288,11 +1191,8 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="E30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>100129</v>
       </c>
@@ -1304,9 +1204,6 @@
       </c>
       <c r="D31" s="7">
         <v>2</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1440,10 +1337,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1494,7 +1391,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,30 +1494,38 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8ECDD-6B59-425A-9189-E22DC1282E23}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1630,41 +1535,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13B9986-6B44-407B-9E7B-E5C69B4870CC}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>100102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7C17CB-17CC-4531-A19C-16586065C374}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1739,7 +1609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAC7ABB-2671-49BC-9122-B2CF83A2CAC4}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add constructing of Student object
</commit_message>
<xml_diff>
--- a/final_project/school_journal/database/excel.xlsx
+++ b/final_project/school_journal/database/excel.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\school_journal\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DC146B-A79E-4A78-B34C-C13AC74C346D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A6F3E3-29EE-42BB-8294-3198F9447865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27720" yWindow="0" windowWidth="22395" windowHeight="13170" tabRatio="790" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-27720" yWindow="0" windowWidth="22395" windowHeight="13170" tabRatio="790" activeTab="3" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
     <sheet name="Courses" sheetId="3" r:id="rId2"/>
     <sheet name="Fields of study" sheetId="2" r:id="rId3"/>
     <sheet name="Grades" sheetId="5" r:id="rId4"/>
-    <sheet name="Grades comments" sheetId="8" r:id="rId5"/>
-    <sheet name="Instructors" sheetId="4" r:id="rId6"/>
-    <sheet name="Enrollments" sheetId="6" r:id="rId7"/>
+    <sheet name="Instructors" sheetId="4" r:id="rId5"/>
+    <sheet name="Enrollments" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>Index</t>
   </si>
@@ -312,12 +311,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Grade_ID</t>
-  </si>
-  <si>
-    <t>Some comment.</t>
-  </si>
-  <si>
     <t>Short_name</t>
   </si>
   <si>
@@ -325,6 +318,18 @@
   </si>
   <si>
     <t>Field_of_study</t>
+  </si>
+  <si>
+    <t>No comment.</t>
+  </si>
+  <si>
+    <t>Bad job :(</t>
+  </si>
+  <si>
+    <t>Aweful work</t>
+  </si>
+  <si>
+    <t>Well done!</t>
   </si>
 </sst>
 </file>
@@ -758,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4C6B96-C4DC-4735-B81E-35A8CA1960AC}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -783,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1337,10 +1342,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1388,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BBAA83-CB17-480D-9BF2-9E6FB44F98AF}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,9 +1405,10 @@
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1415,8 +1421,11 @@
       <c r="D1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1429,8 +1438,11 @@
       <c r="D2" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1443,8 +1455,11 @@
       <c r="D3" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1457,8 +1472,11 @@
       <c r="D4" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1471,8 +1489,11 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1484,6 +1505,9 @@
       </c>
       <c r="D6" s="9">
         <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1493,48 +1517,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D8ECDD-6B59-425A-9189-E22DC1282E23}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7C17CB-17CC-4531-A19C-16586065C374}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1609,7 +1591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAC7ABB-2671-49BC-9122-B2CF83A2CAC4}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add save_to_folder and Instructor creation
</commit_message>
<xml_diff>
--- a/final_project/school_journal/database/excel.xlsx
+++ b/final_project/school_journal/database/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\uni_oop\final_project\school_journal\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06155AA1-32CF-4947-98DD-59E1E996626A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC2CC5E-DCFC-4B33-949C-E66FED3DED8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="-120" windowWidth="27960" windowHeight="16440" tabRatio="790" activeTab="5" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
+    <workbookView xWindow="-27840" yWindow="-120" windowWidth="27960" windowHeight="16440" tabRatio="790" activeTab="1" xr2:uid="{D84FEE5B-BA33-4EFE-AC61-761A747DD1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2E8602-E091-4247-B9B8-7B287103D30F}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,7 +1595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EAC7ABB-2671-49BC-9122-B2CF83A2CAC4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>

</xml_diff>